<commit_message>
adding csv for surface water data; 1/2 det limit for nondetects
</commit_message>
<xml_diff>
--- a/observed_concentrations/cdpr_stormdrain_bifenthrin_09-14_all.xlsx
+++ b/observed_concentrations/cdpr_stormdrain_bifenthrin_09-14_all.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echelsvi\git\yuan_urban_pesticides\observed_concentrations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\yuan_urban_pesticides\observed_concentrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4226FC10-39BC-4587-B78D-7E7717F40ECF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE021D0-BD4F-45A2-974D-85B1D7BBED5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="3045" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25065" yWindow="1500" windowWidth="21600" windowHeight="13995" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2009-14 Water" sheetId="3" r:id="rId1"/>
-    <sheet name="2009-14 Sediment" sheetId="5" r:id="rId2"/>
+    <sheet name="water_data_2009_2014" sheetId="6" r:id="rId2"/>
+    <sheet name="2009-14 Sediment" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2009-14 Sediment'!$A$1:$N$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2009-14 Sediment'!$A$1:$N$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2009-14 Water'!$A$1:$L$80</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="71">
   <si>
     <t>Sample Date</t>
   </si>
@@ -237,6 +238,18 @@
   <si>
     <t>rl</t>
   </si>
+  <si>
+    <t>sample_date</t>
+  </si>
+  <si>
+    <t>site_id</t>
+  </si>
+  <si>
+    <t>detect</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
 </sst>
 </file>
 
@@ -288,7 +301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -326,6 +339,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -333,7 +357,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,6 +397,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E070BE-8C5D-4B68-B77F-40E6DAF2E7CF}">
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4032,6 +4060,1149 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F515302-EB39-46CF-BCD4-D7079BF8EBEF}">
+  <dimension ref="A1:D81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>39857</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>39910</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>39916</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>39934</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2.0300000000000002E-2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>40053</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.6800000000000002E-2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>40053</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1.6800000000000002E-2</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>40098</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>40098</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1.41E-2</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>40099</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>40099</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3.32E-2</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>40272</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>40272</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>40378</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>40475</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>40590</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>40678</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4">
+        <v>6.4799999999999996E-2</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>40721</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>40756</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2.7600000000000003E-2</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>40756</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="4">
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>40757</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="4">
+        <v>7.3799999999999991E-2</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>40757</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2.4399999999999998E-2</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>40821</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1.9399999999999997E-2</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>40821</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="4">
+        <v>9.8499999999999994E-3</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>40821</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="4">
+        <v>5.4100000000000002E-2</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>40821</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="4">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>40928</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="4">
+        <v>4.8600000000000004E-2</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>40928</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1.29E-2</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>40928</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="4">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>40928</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="4">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>41079</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>41079</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1.41E-2</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>41079</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="4">
+        <v>3.5400000000000001E-2</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>41079</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="4">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>41121</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1.3699999999999999E-2</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>41121</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="4">
+        <v>2.4700000000000004E-3</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>41157</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="4">
+        <v>3.3300000000000001E-3</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>41157</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="4">
+        <v>4.15E-3</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>41204</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="4">
+        <v>1.49E-2</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>41204</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>41324</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="4">
+        <v>5.9799999999999999E-2</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>41324</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1.72E-2</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>41324</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>41324</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="4">
+        <v>4.99E-2</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>41394</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>41394</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="4">
+        <v>9.8900000000000012E-3</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>41395</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="4">
+        <v>1.9299999999999999E-3</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>41395</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="4">
+        <v>1.1699999999999999E-2</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>41429</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="4">
+        <v>3.8700000000000002E-3</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>41429</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="4">
+        <v>6.77E-3</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>41429</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="4">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>41429</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="4">
+        <v>8.9700000000000005E-3</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>41464</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="4">
+        <v>3.9899999999999996E-3</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>41464</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" s="4">
+        <v>7.0299999999999998E-3</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>41492</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="4">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>41492</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="4">
+        <v>2.1099999999999999E-3</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>41492</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="4">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>41492</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="4">
+        <v>9.5700000000000004E-3</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>41597</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C59" s="4">
+        <v>8.1600000000000006E-2</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>41597</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="4">
+        <v>6.2700000000000006E-2</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>41597</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="4">
+        <v>3.27E-2</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>41597</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="4">
+        <v>3.6700000000000003E-2</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>41696</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C63" s="4">
+        <v>2.53E-2</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>41696</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C64" s="4">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>41696</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="4">
+        <v>2.6100000000000002E-2</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>41696</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" s="4">
+        <v>2.7300000000000001E-2</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>41715</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="4">
+        <v>5.5118764612361792E-3</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>41715</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" s="4">
+        <v>2.8028748721625446E-2</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>41766</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69" s="4">
+        <v>3.1800000000000001E-3</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>41766</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C70" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>41792</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="4">
+        <v>6.0299999999999998E-3</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>41792</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>41794</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>41794</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C74" s="4">
+        <v>1.09E-2</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>41829</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C75" s="4">
+        <v>2.4299999999999999E-2</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>41829</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" s="4">
+        <v>1.47E-2</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>41857</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" s="4">
+        <v>1.83E-2</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>41857</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C78" s="4">
+        <v>1.29E-2</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>41943</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="4">
+        <v>5.3800000000000001E-2</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>41943</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C80" s="4">
+        <v>0.158</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B35A0B-9AA1-4442-8A46-68B27C9017E9}">
   <dimension ref="A1:N42"/>
   <sheetViews>

</xml_diff>